<commit_message>
Eurorack USB power design added
</commit_message>
<xml_diff>
--- a/Eurorack_MIDIThru4_DIN/Eurorack_MIDIThru4_DIN_bom.xlsx
+++ b/Eurorack_MIDIThru4_DIN/Eurorack_MIDIThru4_DIN_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aokudrya/Documents/GitHub/Midi-boards/Eurorack_MIDIThru4_DIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3C096C-FB6A-4D49-BA1E-B557A5ABCAD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD21F95C-5E29-D74E-A88F-F119ACDE5666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32920" yWindow="2720" windowWidth="28800" windowHeight="16200" xr2:uid="{1DC00C95-4B08-F94A-83B0-76F56463D0E9}"/>
   </bookViews>
@@ -581,9 +581,6 @@
     <t>5-pin DIN connector</t>
   </si>
   <si>
-    <t>MIDI socket</t>
-  </si>
-  <si>
     <t>DIP-14 W7.62mm IC socket round pins</t>
   </si>
   <si>
@@ -712,6 +709,9 @@
   </si>
   <si>
     <t>Power regulator</t>
+  </si>
+  <si>
+    <t>SDS-50J</t>
   </si>
 </sst>
 </file>
@@ -1368,7 +1368,7 @@
   <dimension ref="A1:AJ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="107" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="2" spans="1:29" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1588,7 +1588,7 @@
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19">
@@ -1599,7 +1599,7 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3">
@@ -1749,10 +1749,10 @@
         <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -2211,13 +2211,13 @@
     <row r="27" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
@@ -2324,7 +2324,7 @@
         <v>181</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="E31" s="3">
         <v>5</v>
@@ -2360,10 +2360,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="E32" s="3">
         <v>1</v>
@@ -2399,10 +2399,10 @@
         <v>5</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="E33" s="3">
         <v>1</v>
@@ -2414,10 +2414,10 @@
         <v>46</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="E34" s="3">
         <v>1</v>
@@ -2426,13 +2426,13 @@
     <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="E35" s="3">
         <v>2</v>
@@ -2462,13 +2462,13 @@
     <row r="36" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E36" s="3">
         <v>1</v>
@@ -2477,13 +2477,13 @@
     <row r="37" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="E37" s="3">
         <v>2</v>
@@ -2492,13 +2492,13 @@
     <row r="38" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E38" s="3">
         <v>1</v>
@@ -2507,13 +2507,13 @@
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="E39" s="3">
         <v>15</v>
@@ -2568,7 +2568,7 @@
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2597,7 +2597,7 @@
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3">
@@ -2673,7 +2673,7 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="47" spans="1:29" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
@@ -2772,7 +2772,7 @@
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="51" spans="1:29" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="52" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
@@ -2903,7 +2903,7 @@
     </row>
     <row r="54" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E54" s="7"/>
       <c r="R54" t="s">
@@ -2933,7 +2933,7 @@
     </row>
     <row r="55" spans="1:29" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E55" s="7"/>
     </row>

</xml_diff>

<commit_message>
added Eurorack MIDI Merger 2->3
</commit_message>
<xml_diff>
--- a/Eurorack_MIDIThru4_DIN/Eurorack_MIDIThru4_DIN_bom.xlsx
+++ b/Eurorack_MIDIThru4_DIN/Eurorack_MIDIThru4_DIN_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aokudrya/Documents/GitHub/Midi-boards/Eurorack_MIDIThru4_DIN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrei/Documents/GitHub/Midi-boards/Eurorack_MIDIThru4_DIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD21F95C-5E29-D74E-A88F-F119ACDE5666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BEC794-3AB7-A448-846B-48574CFF85BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32920" yWindow="2720" windowWidth="28800" windowHeight="16200" xr2:uid="{1DC00C95-4B08-F94A-83B0-76F56463D0E9}"/>
   </bookViews>
@@ -650,6 +650,46 @@
     <t xml:space="preserve">* Consider proper orientation for Pin1 IC sockets and polarity for capacitors, diode marks. </t>
   </si>
   <si>
+    <t>* if DC 5.5 barrel jack used for power, JP1 sets external voltage: (1-2) - 5V(also USB cable) 
+  or (2-3): 6-12V</t>
+  </si>
+  <si>
+    <t>* First prototype boards have an ID on the front panel, that's expected, later boards will get it removed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Early boards have a front panel mistake the activity LED for power LED labels </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>IDC 16-Pin connector</t>
+  </si>
+  <si>
+    <t>IDC16</t>
+  </si>
+  <si>
+    <t>ribbon cable</t>
+  </si>
+  <si>
+    <t>1ft 16-pin ribbon cable</t>
+  </si>
+  <si>
+    <t>Screws for DIN connector</t>
+  </si>
+  <si>
+    <t>screw</t>
+  </si>
+  <si>
+    <t>L7805</t>
+  </si>
+  <si>
+    <t>Power regulator</t>
+  </si>
+  <si>
+    <t>SDS-50J</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -669,49 +709,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>. In future versions it will be down. 
+      <t>.
   Set JP2 to use either 5V or 12V power: (1-2) - 5V, (2-3) - 12V</t>
     </r>
-  </si>
-  <si>
-    <t>* if DC 5.5 barrel jack used for power, JP1 sets external voltage: (1-2) - 5V(also USB cable) 
-  or (2-3): 6-12V</t>
-  </si>
-  <si>
-    <t>* First prototype boards have an ID on the front panel, that's expected, later boards will get it removed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Early boards have a front panel mistake the activity LED for power LED labels </t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>IDC 16-Pin connector</t>
-  </si>
-  <si>
-    <t>IDC16</t>
-  </si>
-  <si>
-    <t>ribbon cable</t>
-  </si>
-  <si>
-    <t>1ft 16-pin ribbon cable</t>
-  </si>
-  <si>
-    <t>Screws for DIN connector</t>
-  </si>
-  <si>
-    <t>screw</t>
-  </si>
-  <si>
-    <t>L7805</t>
-  </si>
-  <si>
-    <t>Power regulator</t>
-  </si>
-  <si>
-    <t>SDS-50J</t>
   </si>
 </sst>
 </file>
@@ -891,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -911,15 +911,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1367,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="107" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="107" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1432,13 +1425,13 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="31" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
       <c r="R2" t="s">
         <v>3</v>
       </c>
@@ -1584,14 +1577,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1728,7 +1721,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
@@ -1749,10 +1742,10 @@
         <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -2208,7 +2201,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>194</v>
@@ -2324,7 +2317,7 @@
         <v>181</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E31" s="3">
         <v>5</v>
@@ -2393,7 +2386,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -2408,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>46</v>
@@ -2459,7 +2452,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
         <v>201</v>
@@ -2474,31 +2467,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="E37" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E38" s="3">
         <v>1</v>
@@ -2507,13 +2500,13 @@
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="E39" s="3">
         <v>15</v>
@@ -2672,7 +2665,7 @@
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="14" t="s">
         <v>187</v>
       </c>
       <c r="B45" s="5"/>
@@ -2699,18 +2692,15 @@
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="16"/>
+      <c r="A46" s="13"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:29" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
       <c r="E47" s="7"/>
       <c r="R47" t="s">
         <v>13</v>
@@ -2738,13 +2728,13 @@
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="28"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="23"/>
       <c r="R48" t="s">
         <v>13</v>
       </c>
@@ -2771,12 +2761,12 @@
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A49" s="21" t="s">
+      <c r="A49" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
       <c r="E49" s="8"/>
       <c r="R49" t="s">
         <v>13</v>
@@ -2801,13 +2791,13 @@
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A50" s="21" t="s">
+      <c r="A50" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="28"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="23"/>
       <c r="R50" t="s">
         <v>13</v>
       </c>
@@ -2831,20 +2821,20 @@
       </c>
     </row>
     <row r="51" spans="1:29" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="21" t="s">
+      <c r="A51" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="13"/>
-    </row>
-    <row r="52" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
       <c r="E52" s="7"/>
       <c r="R52" t="s">
         <v>13</v>
@@ -2872,9 +2862,9 @@
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A53" s="23"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
+      <c r="A53" s="18"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
       <c r="E53" s="7"/>
       <c r="R53" t="s">
         <v>13</v>
@@ -2903,7 +2893,7 @@
     </row>
     <row r="54" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E54" s="7"/>
       <c r="R54" t="s">
@@ -2931,14 +2921,14 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:29" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="20"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>

</xml_diff>